<commit_message>
Data and figure organization
</commit_message>
<xml_diff>
--- a/data/HIV/T-cell-intensity/T cell intensity.xlsx
+++ b/data/HIV/T-cell-intensity/T cell intensity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiruigao/Desktop/paper-time-varying-selection/data/HIV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiruigao/Desktop/paper-time-varying-selection/data/HIV/T-cell-intensity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB72CB-BD98-FF4A-9992-506F6E78BE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D2DC78-671E-B444-BF63-FFE0AC1EB1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1440" windowWidth="29920" windowHeight="17360" xr2:uid="{382D3FFB-DD9D-BB43-8D38-AE167FFEBC03}"/>
+    <workbookView xWindow="320" yWindow="1080" windowWidth="29920" windowHeight="17360" xr2:uid="{382D3FFB-DD9D-BB43-8D38-AE167FFEBC03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="194">
   <si>
     <t>Gag147-155</t>
   </si>
@@ -578,9 +578,6 @@
     <t>Gag71-79</t>
   </si>
   <si>
-    <t>Env838-854</t>
-  </si>
-  <si>
     <t>GTEELRSLY</t>
   </si>
   <si>
@@ -588,13 +585,46 @@
   </si>
   <si>
     <t>TSTLQEQVAW</t>
+  </si>
+  <si>
+    <t>KAAFDLSFF</t>
+  </si>
+  <si>
+    <t>EL9</t>
+  </si>
+  <si>
+    <t>ERYLRDQQL</t>
+  </si>
+  <si>
+    <t>DLLKTVRLI</t>
+  </si>
+  <si>
+    <t>DI9</t>
+  </si>
+  <si>
+    <t>TLSHVVDKL</t>
+  </si>
+  <si>
+    <t>TL9</t>
+  </si>
+  <si>
+    <t>DRVIEELQR</t>
+  </si>
+  <si>
+    <t>nef</t>
+  </si>
+  <si>
+    <t>KRREILDLWVY</t>
+  </si>
+  <si>
+    <t>KY11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -618,6 +648,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -659,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -702,6 +745,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C60953-7627-3A4A-BE53-D130D055A2D5}">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1237,7 @@
       <c r="G6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="9">
@@ -1261,7 +1310,7 @@
       <c r="G8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="9">
@@ -1278,95 +1327,74 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="10">
+        <v>700010077</v>
+      </c>
+      <c r="E9">
+        <v>6000</v>
+      </c>
+      <c r="F9">
+        <v>6026</v>
+      </c>
+      <c r="G9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I10" s="9">
+      <c r="A10" s="10">
+        <v>700010077</v>
+      </c>
+      <c r="E10">
+        <v>7245</v>
+      </c>
+      <c r="F10">
+        <v>7271</v>
+      </c>
+      <c r="G10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>700010077</v>
+      </c>
+      <c r="E11">
+        <v>8703</v>
+      </c>
+      <c r="F11">
+        <v>8729</v>
+      </c>
+      <c r="G11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I12" s="9">
         <v>16</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J12" s="9">
         <v>45</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K12" s="9">
         <v>111</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L12" s="9">
         <v>181</v>
       </c>
-      <c r="M10" s="9">
-        <v>266</v>
-      </c>
-      <c r="N10" s="9">
+      <c r="M12" s="9">
+        <v>283</v>
+      </c>
+      <c r="N12" s="9">
         <v>412</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>700010040</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1972</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1998</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1972</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1998</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="9">
-        <v>97.46</v>
-      </c>
-      <c r="J11" s="9">
-        <v>65.349999999999994</v>
-      </c>
-      <c r="K11" s="9">
-        <v>164.68</v>
-      </c>
-      <c r="L11" s="9">
-        <v>74.31</v>
-      </c>
-      <c r="M11" s="9">
-        <v>94.94</v>
-      </c>
-      <c r="N11" s="9">
-        <v>98.95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>700010040</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="9">
-        <v>2230</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2283</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2230</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2256</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1374,22 +1402,43 @@
         <v>700010040</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13" s="9">
-        <v>2325</v>
+        <v>1972</v>
       </c>
       <c r="D13" s="9">
-        <v>2378</v>
+        <v>1998</v>
       </c>
       <c r="E13" s="1">
-        <v>2352</v>
+        <v>1972</v>
       </c>
       <c r="F13" s="1">
-        <v>2378</v>
+        <v>1998</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="9">
+        <v>97.46</v>
+      </c>
+      <c r="J13" s="9">
+        <v>65.349999999999994</v>
+      </c>
+      <c r="K13" s="9">
+        <v>164.68</v>
+      </c>
+      <c r="L13" s="9">
+        <v>74.31</v>
+      </c>
+      <c r="M13" s="9">
+        <v>94.94</v>
+      </c>
+      <c r="N13" s="9">
+        <v>98.95</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1397,112 +1446,115 @@
         <v>700010040</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="9">
-        <v>4557</v>
+        <v>2230</v>
       </c>
       <c r="D14" s="9">
-        <v>4610</v>
+        <v>2283</v>
       </c>
       <c r="E14" s="2">
-        <v>4569</v>
+        <v>2230</v>
       </c>
       <c r="F14" s="2">
-        <v>4595</v>
+        <v>2256</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>700010040</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="9">
-        <v>5395</v>
+        <v>2325</v>
       </c>
       <c r="D15" s="9">
-        <v>5421</v>
+        <v>2378</v>
       </c>
       <c r="E15" s="1">
-        <v>5395</v>
+        <v>2352</v>
       </c>
       <c r="F15" s="1">
-        <v>5421</v>
+        <v>2378</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="9">
-        <v>139.28</v>
-      </c>
-      <c r="J15" s="9">
-        <v>213.97</v>
-      </c>
-      <c r="K15" s="9">
-        <v>396.19</v>
-      </c>
-      <c r="L15" s="9">
-        <v>66.84</v>
-      </c>
-      <c r="M15" s="9">
-        <v>275.67</v>
-      </c>
-      <c r="N15" s="9">
-        <v>98.95</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>700010040</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="9">
-        <v>8447</v>
+        <v>4557</v>
       </c>
       <c r="D16" s="9">
-        <v>8500</v>
+        <v>4610</v>
       </c>
       <c r="E16" s="2">
-        <v>8471</v>
+        <v>4569</v>
       </c>
       <c r="F16" s="2">
-        <v>8497</v>
+        <v>4595</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>700010040</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="9">
-        <v>8517</v>
+        <v>5395</v>
       </c>
       <c r="D17" s="9">
-        <v>8575</v>
-      </c>
-      <c r="E17" s="2">
-        <v>8532</v>
-      </c>
-      <c r="F17" s="2">
-        <v>8558</v>
+        <v>5421</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5395</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5421</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="9">
+        <v>139.28</v>
+      </c>
+      <c r="J17" s="9">
+        <v>213.97</v>
+      </c>
+      <c r="K17" s="9">
+        <v>396.19</v>
+      </c>
+      <c r="L17" s="9">
+        <v>66.84</v>
+      </c>
+      <c r="M17" s="9">
+        <v>275.67</v>
+      </c>
+      <c r="N17" s="9">
+        <v>98.95</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1510,150 +1562,152 @@
         <v>700010040</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C18" s="9">
-        <v>8712</v>
+        <v>8447</v>
       </c>
       <c r="D18" s="9">
-        <v>8765</v>
+        <v>8500</v>
       </c>
       <c r="E18" s="2">
-        <v>8727</v>
+        <v>8471</v>
       </c>
       <c r="F18" s="2">
-        <v>8753</v>
+        <v>8497</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="9">
-        <v>22.78</v>
-      </c>
-      <c r="J18" s="9">
-        <v>89.25</v>
-      </c>
-      <c r="K18" s="9">
-        <v>257.27999999999997</v>
-      </c>
-      <c r="L18" s="9">
-        <v>98.2</v>
-      </c>
-      <c r="M18" s="9">
-        <v>206.22</v>
-      </c>
-      <c r="N18" s="9">
-        <v>37.71</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>700010040</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="9">
+        <v>8517</v>
+      </c>
+      <c r="D19" s="9">
+        <v>8575</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8532</v>
+      </c>
+      <c r="F19" s="2">
+        <v>8558</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>700010040</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="9">
+        <v>8712</v>
+      </c>
+      <c r="D20" s="9">
+        <v>8765</v>
+      </c>
+      <c r="E20" s="2">
+        <v>8727</v>
+      </c>
+      <c r="F20" s="2">
+        <v>8753</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="9">
+        <v>22.78</v>
+      </c>
+      <c r="J20" s="9">
+        <v>89.25</v>
+      </c>
+      <c r="K20" s="9">
+        <v>257.27999999999997</v>
+      </c>
+      <c r="L20" s="9">
+        <v>98.2</v>
+      </c>
+      <c r="M20" s="9">
+        <v>206.22</v>
+      </c>
+      <c r="N20" s="9">
+        <v>37.71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>700010040</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C21" s="9">
         <v>9355</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D21" s="9">
         <v>9384</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E21" s="1">
         <v>9355</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F21" s="1">
         <v>9384</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I21" s="9">
         <v>140.78</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J21" s="9">
         <v>7.84</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K21" s="9">
         <v>19.8</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L21" s="9">
         <v>8.59</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M21" s="9">
         <v>19.510000000000002</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N21" s="9">
         <v>22.78</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I21" s="9">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I23" s="9">
         <v>33</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J23" s="9">
         <v>47</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K23" s="9">
         <v>112</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L23" s="9">
         <v>186</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M23" s="9">
         <v>356</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
-        <v>705010162</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1054</v>
-      </c>
-      <c r="D22" s="9">
-        <v>1083</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1051</v>
-      </c>
-      <c r="F22" s="4">
-        <v>1077</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
-        <v>705010162</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="9">
-        <v>1954</v>
-      </c>
-      <c r="D23" s="9">
-        <v>2007</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1975</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2001</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -1661,22 +1715,22 @@
         <v>705010162</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="9">
-        <v>2352</v>
+        <v>1054</v>
       </c>
       <c r="D24" s="9">
-        <v>2378</v>
-      </c>
-      <c r="E24" s="1">
-        <v>2352</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2378</v>
+        <v>1083</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1051</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1077</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1684,22 +1738,22 @@
         <v>705010162</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25" s="9">
-        <v>4197</v>
+        <v>1954</v>
       </c>
       <c r="D25" s="9">
-        <v>4250</v>
+        <v>2007</v>
       </c>
       <c r="E25" s="2">
-        <v>4203</v>
+        <v>1975</v>
       </c>
       <c r="F25" s="2">
-        <v>4229</v>
+        <v>2001</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1707,22 +1761,22 @@
         <v>705010162</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C26" s="9">
-        <v>5368</v>
+        <v>2352</v>
       </c>
       <c r="D26" s="9">
-        <v>5394</v>
+        <v>2378</v>
       </c>
       <c r="E26" s="1">
-        <v>5368</v>
+        <v>2352</v>
       </c>
       <c r="F26" s="1">
-        <v>5394</v>
+        <v>2378</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -1730,37 +1784,22 @@
         <v>705010162</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C27" s="9">
-        <v>5994</v>
+        <v>4197</v>
       </c>
       <c r="D27" s="9">
-        <v>6044</v>
+        <v>4250</v>
       </c>
       <c r="E27" s="2">
-        <v>6006</v>
+        <v>4203</v>
       </c>
       <c r="F27" s="2">
-        <v>6032</v>
+        <v>4229</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J27" s="9">
-        <v>1.17</v>
-      </c>
-      <c r="K27" s="9">
-        <v>400</v>
-      </c>
-      <c r="L27" s="9">
-        <v>5.08</v>
-      </c>
-      <c r="M27" s="9">
-        <v>36.33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -1768,40 +1807,22 @@
         <v>705010162</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C28" s="9">
-        <v>8845</v>
+        <v>5368</v>
       </c>
       <c r="D28" s="9">
-        <v>8898</v>
-      </c>
-      <c r="E28" s="2">
-        <v>8851</v>
-      </c>
-      <c r="F28" s="2">
-        <v>8877</v>
+        <v>5394</v>
+      </c>
+      <c r="E28" s="1">
+        <v>5368</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5394</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="9">
-        <v>50.39</v>
-      </c>
-      <c r="J28" s="9">
-        <v>137.11000000000001</v>
-      </c>
-      <c r="K28" s="9">
-        <v>206.45</v>
-      </c>
-      <c r="L28" s="9">
-        <v>12.89</v>
-      </c>
-      <c r="M28" s="9">
-        <v>19.920000000000002</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1809,22 +1830,37 @@
         <v>705010162</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" s="9">
-        <v>8968</v>
+        <v>5994</v>
       </c>
       <c r="D29" s="9">
-        <v>9042</v>
+        <v>6044</v>
       </c>
       <c r="E29" s="2">
-        <v>9007</v>
+        <v>6006</v>
       </c>
       <c r="F29" s="2">
-        <v>9033</v>
+        <v>6032</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="9">
+        <v>1.17</v>
+      </c>
+      <c r="K29" s="9">
+        <v>400</v>
+      </c>
+      <c r="L29" s="9">
+        <v>5.08</v>
+      </c>
+      <c r="M29" s="9">
+        <v>36.33</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1832,106 +1868,125 @@
         <v>705010162</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C30" s="9">
-        <v>9109</v>
+        <v>8845</v>
       </c>
       <c r="D30" s="9">
-        <v>9162</v>
+        <v>8898</v>
       </c>
       <c r="E30" s="2">
-        <v>9118</v>
+        <v>8851</v>
       </c>
       <c r="F30" s="2">
-        <v>9144</v>
+        <v>8877</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I30" s="9">
-        <v>141.02000000000001</v>
+        <v>50.39</v>
       </c>
       <c r="J30" s="9">
-        <v>283.87</v>
+        <v>137.11000000000001</v>
       </c>
       <c r="K30" s="9">
-        <v>696.77</v>
+        <v>206.45</v>
       </c>
       <c r="L30" s="9">
-        <v>28.52</v>
+        <v>12.89</v>
       </c>
       <c r="M30" s="9">
-        <v>14.45</v>
+        <v>19.920000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I31" s="9">
-        <v>7</v>
-      </c>
-      <c r="J31" s="9">
-        <v>28</v>
-      </c>
-      <c r="K31" s="9">
-        <v>34</v>
-      </c>
-      <c r="L31" s="9">
-        <v>63</v>
-      </c>
-      <c r="M31" s="9">
-        <v>91</v>
-      </c>
-      <c r="N31" s="9">
-        <v>120</v>
-      </c>
+      <c r="A31" s="12">
+        <v>705010162</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="9">
+        <v>8968</v>
+      </c>
+      <c r="D31" s="9">
+        <v>9042</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9007</v>
+      </c>
+      <c r="F31" s="2">
+        <v>9033</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
-        <v>703010256</v>
+        <v>705010162</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C32" s="9">
-        <v>1207</v>
+        <v>9109</v>
       </c>
       <c r="D32" s="9">
-        <v>1260</v>
+        <v>9162</v>
       </c>
       <c r="E32" s="2">
-        <v>1210</v>
+        <v>9118</v>
       </c>
       <c r="F32" s="2">
-        <v>1239</v>
+        <v>9144</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="9">
+        <v>141.02000000000001</v>
+      </c>
+      <c r="J32" s="9">
+        <v>283.87</v>
+      </c>
+      <c r="K32" s="9">
+        <v>696.77</v>
+      </c>
+      <c r="L32" s="9">
+        <v>28.52</v>
+      </c>
+      <c r="M32" s="9">
+        <v>14.45</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="12">
-        <v>703010256</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="9">
-        <v>1663</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1716</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1681</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1707</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>67</v>
+      <c r="I33" s="9">
+        <v>7</v>
+      </c>
+      <c r="J33" s="9">
+        <v>28</v>
+      </c>
+      <c r="K33" s="9">
+        <v>34</v>
+      </c>
+      <c r="L33" s="9">
+        <v>63</v>
+      </c>
+      <c r="M33" s="9">
+        <v>91</v>
+      </c>
+      <c r="N33" s="9">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -1939,43 +1994,22 @@
         <v>703010256</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C34" s="9">
-        <v>3261</v>
+        <v>1207</v>
       </c>
       <c r="D34" s="9">
-        <v>3314</v>
+        <v>1260</v>
       </c>
       <c r="E34" s="2">
-        <v>3276</v>
+        <v>1210</v>
       </c>
       <c r="F34" s="2">
-        <v>3302</v>
+        <v>1239</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I34" s="9">
-        <v>0</v>
-      </c>
-      <c r="J34" s="9">
-        <v>8.23</v>
-      </c>
-      <c r="K34" s="9">
-        <v>43.41</v>
-      </c>
-      <c r="L34" s="9">
-        <v>115.92</v>
-      </c>
-      <c r="M34" s="9">
-        <v>155.32</v>
-      </c>
-      <c r="N34" s="9">
-        <v>496.68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -1983,22 +2017,22 @@
         <v>703010256</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C35" s="9">
-        <v>3861</v>
+        <v>1663</v>
       </c>
       <c r="D35" s="9">
-        <v>3914</v>
+        <v>1716</v>
       </c>
       <c r="E35" s="2">
-        <v>3888</v>
+        <v>1681</v>
       </c>
       <c r="F35" s="2">
-        <v>3914</v>
+        <v>1707</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -2006,43 +2040,43 @@
         <v>703010256</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C36" s="9">
-        <v>5545</v>
+        <v>3261</v>
       </c>
       <c r="D36" s="9">
-        <v>5598</v>
+        <v>3314</v>
       </c>
       <c r="E36" s="2">
-        <v>5551</v>
+        <v>3276</v>
       </c>
       <c r="F36" s="2">
-        <v>5577</v>
+        <v>3302</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="I36" s="9">
         <v>0</v>
       </c>
       <c r="J36" s="9">
-        <v>0</v>
+        <v>8.23</v>
       </c>
       <c r="K36" s="9">
-        <v>4.43</v>
+        <v>43.41</v>
       </c>
       <c r="L36" s="9">
-        <v>308.77999999999997</v>
+        <v>115.92</v>
       </c>
       <c r="M36" s="9">
-        <v>13.11</v>
+        <v>155.32</v>
       </c>
       <c r="N36" s="9">
-        <v>175.24</v>
+        <v>496.68</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -2050,45 +2084,67 @@
         <v>703010256</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C37" s="9">
-        <v>5834</v>
+        <v>3861</v>
       </c>
       <c r="D37" s="9">
-        <v>5863</v>
-      </c>
-      <c r="E37" s="1">
-        <v>5834</v>
-      </c>
-      <c r="F37" s="1">
-        <v>5863</v>
+        <v>3914</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3888</v>
+      </c>
+      <c r="F37" s="2">
+        <v>3914</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>77</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>703010256</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C38" s="9">
-        <v>8040</v>
+        <v>5545</v>
       </c>
       <c r="D38" s="9">
-        <v>8072</v>
+        <v>5598</v>
       </c>
       <c r="E38" s="2">
-        <v>8040</v>
+        <v>5551</v>
       </c>
       <c r="F38" s="2">
-        <v>8066</v>
+        <v>5577</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I38" s="9">
+        <v>0</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0</v>
+      </c>
+      <c r="K38" s="9">
+        <v>4.43</v>
+      </c>
+      <c r="L38" s="9">
+        <v>308.77999999999997</v>
+      </c>
+      <c r="M38" s="9">
+        <v>13.11</v>
+      </c>
+      <c r="N38" s="9">
+        <v>175.24</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -2096,203 +2152,172 @@
         <v>703010256</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C39" s="9">
-        <v>8445</v>
+        <v>5834</v>
       </c>
       <c r="D39" s="9">
-        <v>8498</v>
-      </c>
-      <c r="E39" s="2">
-        <v>8448</v>
-      </c>
-      <c r="F39" s="2">
-        <v>8474</v>
+        <v>5863</v>
+      </c>
+      <c r="E39" s="1">
+        <v>5834</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5863</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="I39" s="9">
-        <v>23.48</v>
-      </c>
-      <c r="J39" s="9">
-        <v>799.57</v>
-      </c>
-      <c r="K39" s="9">
-        <v>64.83</v>
-      </c>
-      <c r="L39" s="9">
-        <v>18.510000000000002</v>
-      </c>
-      <c r="M39" s="9">
-        <v>9.2100000000000009</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <v>703010256</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C40" s="9">
-        <v>8619</v>
+        <v>8040</v>
       </c>
       <c r="D40" s="9">
-        <v>8645</v>
-      </c>
-      <c r="E40" s="1">
-        <v>8619</v>
-      </c>
-      <c r="F40" s="1">
-        <v>8645</v>
+        <v>8072</v>
+      </c>
+      <c r="E40" s="2">
+        <v>8040</v>
+      </c>
+      <c r="F40" s="2">
+        <v>8066</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J40" s="9">
-        <v>919.46</v>
-      </c>
-      <c r="K40" s="9">
-        <v>1017.87</v>
-      </c>
-      <c r="L40" s="9">
-        <v>1934.62</v>
-      </c>
-      <c r="M40" s="9">
-        <v>1608.86</v>
-      </c>
-      <c r="N40" s="9">
-        <v>1381.25</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="12">
         <v>703010256</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C41" s="9">
-        <v>9349</v>
+        <v>8445</v>
       </c>
       <c r="D41" s="9">
-        <v>9402</v>
+        <v>8498</v>
       </c>
       <c r="E41" s="2">
-        <v>9358</v>
+        <v>8448</v>
       </c>
       <c r="F41" s="2">
-        <v>9384</v>
+        <v>8474</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="9">
+        <v>23.48</v>
+      </c>
+      <c r="J41" s="9">
+        <v>799.57</v>
+      </c>
+      <c r="K41" s="9">
+        <v>64.83</v>
+      </c>
+      <c r="L41" s="9">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="M41" s="9">
+        <v>9.2100000000000009</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I42" s="9">
-        <v>24</v>
+      <c r="A42" s="12">
+        <v>703010256</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="9">
+        <v>8619</v>
+      </c>
+      <c r="D42" s="9">
+        <v>8645</v>
+      </c>
+      <c r="E42" s="1">
+        <v>8619</v>
+      </c>
+      <c r="F42" s="1">
+        <v>8645</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="J42" s="9">
-        <v>52</v>
+        <v>919.46</v>
       </c>
       <c r="K42" s="9">
-        <v>80</v>
+        <v>1017.87</v>
       </c>
       <c r="L42" s="9">
-        <v>94</v>
+        <v>1934.62</v>
       </c>
       <c r="M42" s="9">
-        <v>136</v>
+        <v>1608.86</v>
       </c>
       <c r="N42" s="9">
-        <v>185</v>
+        <v>1381.25</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
-        <v>700010470</v>
+        <v>703010256</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" s="9">
-        <v>847</v>
+        <v>9349</v>
       </c>
       <c r="D43" s="9">
-        <v>876</v>
+        <v>9402</v>
       </c>
       <c r="E43" s="2">
-        <v>859</v>
+        <v>9358</v>
       </c>
       <c r="F43" s="2">
-        <v>885</v>
+        <v>9384</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I43" s="9">
-        <v>66.75</v>
-      </c>
-      <c r="K43" s="9">
-        <v>36.65</v>
-      </c>
-      <c r="M43" s="9">
-        <v>564.01</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="12">
-        <v>700010470</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="9">
-        <v>1066</v>
-      </c>
-      <c r="D44" s="9">
-        <v>1092</v>
-      </c>
-      <c r="E44" s="1">
-        <v>1066</v>
-      </c>
-      <c r="F44" s="1">
-        <v>1092</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="I44" s="9">
-        <v>23.56</v>
+        <v>24</v>
       </c>
       <c r="J44" s="9">
-        <v>20.94</v>
+        <v>52</v>
       </c>
       <c r="K44" s="9">
-        <v>289.75</v>
+        <v>80</v>
       </c>
       <c r="L44" s="9">
-        <v>428.51</v>
+        <v>94</v>
       </c>
       <c r="M44" s="9">
-        <v>942.34</v>
+        <v>136</v>
       </c>
       <c r="N44" s="9">
-        <v>770.36</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -2300,31 +2325,34 @@
         <v>700010470</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C45" s="9">
-        <v>2233</v>
+        <v>847</v>
       </c>
       <c r="D45" s="9">
-        <v>2259</v>
-      </c>
-      <c r="E45" s="1">
-        <v>2233</v>
-      </c>
-      <c r="F45" s="1">
-        <v>2259</v>
+        <v>876</v>
+      </c>
+      <c r="E45" s="2">
+        <v>859</v>
+      </c>
+      <c r="F45" s="2">
+        <v>885</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>75</v>
+        <v>89</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="9">
+        <v>66.75</v>
+      </c>
+      <c r="K45" s="9">
+        <v>36.65</v>
       </c>
       <c r="M45" s="9">
-        <v>324.60000000000002</v>
-      </c>
-      <c r="N45" s="9">
-        <v>166.96</v>
+        <v>564.01</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2332,22 +2360,43 @@
         <v>700010470</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C46" s="9">
-        <v>3354</v>
+        <v>1066</v>
       </c>
       <c r="D46" s="9">
-        <v>3380</v>
+        <v>1092</v>
       </c>
       <c r="E46" s="1">
-        <v>3354</v>
+        <v>1066</v>
       </c>
       <c r="F46" s="1">
-        <v>3380</v>
+        <v>1092</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46" s="9">
+        <v>23.56</v>
+      </c>
+      <c r="J46" s="9">
+        <v>20.94</v>
+      </c>
+      <c r="K46" s="9">
+        <v>289.75</v>
+      </c>
+      <c r="L46" s="9">
+        <v>428.51</v>
+      </c>
+      <c r="M46" s="9">
+        <v>942.34</v>
+      </c>
+      <c r="N46" s="9">
+        <v>770.36</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2355,40 +2404,31 @@
         <v>700010470</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C47" s="9">
-        <v>3930</v>
+        <v>2233</v>
       </c>
       <c r="D47" s="9">
-        <v>3956</v>
+        <v>2259</v>
       </c>
       <c r="E47" s="1">
-        <v>3930</v>
+        <v>2233</v>
       </c>
       <c r="F47" s="1">
-        <v>3956</v>
+        <v>2259</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I47" s="9">
-        <v>26.18</v>
-      </c>
-      <c r="J47" s="9">
-        <v>2.62</v>
-      </c>
-      <c r="L47" s="9">
-        <v>596.99</v>
+        <v>95</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="M47" s="9">
-        <v>469.43</v>
+        <v>324.60000000000002</v>
       </c>
       <c r="N47" s="9">
-        <v>201.57</v>
+        <v>166.96</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -2396,63 +2436,64 @@
         <v>700010470</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C48" s="9">
-        <v>5089</v>
+        <v>3354</v>
       </c>
       <c r="D48" s="9">
-        <v>5118</v>
+        <v>3380</v>
       </c>
       <c r="E48" s="1">
-        <v>5089</v>
+        <v>3354</v>
       </c>
       <c r="F48" s="1">
-        <v>5118</v>
+        <v>3380</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I48" s="9">
-        <v>103.4</v>
-      </c>
-      <c r="J48" s="9">
-        <v>3.93</v>
-      </c>
-      <c r="L48" s="9">
-        <v>94.24</v>
-      </c>
-      <c r="M48" s="9">
-        <v>19.63</v>
-      </c>
-      <c r="N48" s="9">
-        <v>10.47</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="12">
         <v>700010470</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C49" s="9">
-        <v>5497</v>
+        <v>3930</v>
       </c>
       <c r="D49" s="9">
-        <v>5550</v>
-      </c>
-      <c r="E49" s="2">
-        <v>5497</v>
-      </c>
-      <c r="F49" s="2">
-        <v>5523</v>
+        <v>3956</v>
+      </c>
+      <c r="E49" s="1">
+        <v>3930</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3956</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I49" s="9">
+        <v>26.18</v>
+      </c>
+      <c r="J49" s="9">
+        <v>2.62</v>
+      </c>
+      <c r="L49" s="9">
+        <v>596.99</v>
+      </c>
+      <c r="M49" s="9">
+        <v>469.43</v>
+      </c>
+      <c r="N49" s="9">
+        <v>201.57</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -2460,22 +2501,40 @@
         <v>700010470</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C50" s="9">
-        <v>8766</v>
+        <v>5089</v>
       </c>
       <c r="D50" s="9">
-        <v>8792</v>
+        <v>5118</v>
       </c>
       <c r="E50" s="1">
-        <v>8766</v>
+        <v>5089</v>
       </c>
       <c r="F50" s="1">
-        <v>8792</v>
+        <v>5118</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I50" s="9">
+        <v>103.4</v>
+      </c>
+      <c r="J50" s="9">
+        <v>3.93</v>
+      </c>
+      <c r="L50" s="9">
+        <v>94.24</v>
+      </c>
+      <c r="M50" s="9">
+        <v>19.63</v>
+      </c>
+      <c r="N50" s="9">
+        <v>10.47</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -2483,144 +2542,129 @@
         <v>700010470</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C51" s="9">
-        <v>8989</v>
+        <v>5497</v>
       </c>
       <c r="D51" s="9">
-        <v>9042</v>
+        <v>5550</v>
       </c>
       <c r="E51" s="2">
-        <v>9016</v>
+        <v>5497</v>
       </c>
       <c r="F51" s="2">
-        <v>9042</v>
+        <v>5523</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>109</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="12">
         <v>700010470</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C52" s="9">
-        <v>9349</v>
+        <v>8766</v>
       </c>
       <c r="D52" s="9">
-        <v>9402</v>
-      </c>
-      <c r="E52" s="2">
-        <v>9358</v>
-      </c>
-      <c r="F52" s="2">
-        <v>9390</v>
+        <v>8792</v>
+      </c>
+      <c r="E52" s="1">
+        <v>8766</v>
+      </c>
+      <c r="F52" s="1">
+        <v>8792</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I52" s="9">
-        <v>10.47</v>
-      </c>
-      <c r="J52" s="9">
-        <v>66.75</v>
-      </c>
-      <c r="L52" s="9">
-        <v>13.09</v>
-      </c>
-      <c r="M52" s="9">
-        <v>61.52</v>
-      </c>
-      <c r="N52" s="9">
-        <v>48.43</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I53" s="9">
-        <v>15</v>
-      </c>
-      <c r="J53" s="9">
-        <v>31</v>
-      </c>
-      <c r="K53" s="9">
-        <v>43</v>
-      </c>
-      <c r="L53" s="9">
-        <v>71</v>
-      </c>
-      <c r="M53" s="9">
-        <v>183</v>
-      </c>
+      <c r="A53" s="12">
+        <v>700010470</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="9">
+        <v>8989</v>
+      </c>
+      <c r="D53" s="9">
+        <v>9042</v>
+      </c>
+      <c r="E53" s="2">
+        <v>9016</v>
+      </c>
+      <c r="F53" s="2">
+        <v>9042</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="12">
-        <v>704010042</v>
+        <v>700010470</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C54" s="9">
-        <v>1183</v>
+        <v>9349</v>
       </c>
       <c r="D54" s="9">
-        <v>1236</v>
+        <v>9402</v>
       </c>
       <c r="E54" s="2">
-        <v>1210</v>
+        <v>9358</v>
       </c>
       <c r="F54" s="2">
-        <v>1236</v>
+        <v>9390</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="I54" s="9">
-        <v>17.61</v>
+        <v>10.47</v>
       </c>
       <c r="J54" s="9">
-        <v>35.21</v>
-      </c>
-      <c r="K54" s="9">
-        <v>147.88999999999999</v>
+        <v>66.75</v>
       </c>
       <c r="L54" s="9">
-        <v>0</v>
+        <v>13.09</v>
       </c>
       <c r="M54" s="9">
-        <v>1</v>
+        <v>61.52</v>
+      </c>
+      <c r="N54" s="9">
+        <v>48.43</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" s="12">
-        <v>704010042</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C55" s="9">
-        <v>2949</v>
-      </c>
-      <c r="D55" s="9">
-        <v>3002</v>
-      </c>
-      <c r="E55" s="2">
-        <v>2958</v>
-      </c>
-      <c r="F55" s="2">
-        <v>2984</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>116</v>
+      <c r="I55" s="9">
+        <v>15</v>
+      </c>
+      <c r="J55" s="9">
+        <v>31</v>
+      </c>
+      <c r="K55" s="9">
+        <v>43</v>
+      </c>
+      <c r="L55" s="9">
+        <v>71</v>
+      </c>
+      <c r="M55" s="9">
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -2628,37 +2672,40 @@
         <v>704010042</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C56" s="9">
-        <v>5994</v>
+        <v>1183</v>
       </c>
       <c r="D56" s="9">
-        <v>6020</v>
-      </c>
-      <c r="E56" s="1">
-        <v>5994</v>
-      </c>
-      <c r="F56" s="1">
-        <v>6020</v>
+        <v>1236</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1210</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1236</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="I56" s="9">
-        <v>3746.34</v>
+        <v>17.61</v>
       </c>
       <c r="J56" s="9">
-        <v>3258.54</v>
+        <v>35.21</v>
+      </c>
+      <c r="K56" s="9">
+        <v>147.88999999999999</v>
       </c>
       <c r="L56" s="9">
-        <v>602.11</v>
+        <v>0</v>
       </c>
       <c r="M56" s="9">
-        <v>59.86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -2666,63 +2713,61 @@
         <v>704010042</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C57" s="9">
-        <v>6729</v>
+        <v>2949</v>
       </c>
       <c r="D57" s="9">
-        <v>6758</v>
+        <v>3002</v>
       </c>
       <c r="E57" s="2">
-        <v>6732</v>
+        <v>2958</v>
       </c>
       <c r="F57" s="2">
-        <v>6758</v>
+        <v>2984</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I57" s="9">
-        <v>669.01</v>
-      </c>
-      <c r="J57" s="9">
-        <v>38.729999999999997</v>
-      </c>
-      <c r="K57" s="9">
-        <v>1229.27</v>
-      </c>
-      <c r="L57" s="9">
-        <v>429.58</v>
-      </c>
-      <c r="M57" s="9">
-        <v>235.92</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="12">
         <v>704010042</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C58" s="9">
-        <v>8133</v>
+        <v>5994</v>
       </c>
       <c r="D58" s="9">
-        <v>8186</v>
-      </c>
-      <c r="E58" s="2">
-        <v>8133</v>
-      </c>
-      <c r="F58" s="2">
-        <v>8159</v>
+        <v>6020</v>
+      </c>
+      <c r="E58" s="1">
+        <v>5994</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6020</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I58" s="9">
+        <v>3746.34</v>
+      </c>
+      <c r="J58" s="9">
+        <v>3258.54</v>
+      </c>
+      <c r="L58" s="9">
+        <v>602.11</v>
+      </c>
+      <c r="M58" s="9">
+        <v>59.86</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -2730,124 +2775,122 @@
         <v>704010042</v>
       </c>
       <c r="B59" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="9">
+        <v>6729</v>
+      </c>
+      <c r="D59" s="9">
+        <v>6758</v>
+      </c>
+      <c r="E59" s="2">
+        <v>6732</v>
+      </c>
+      <c r="F59" s="2">
+        <v>6758</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I59" s="9">
+        <v>669.01</v>
+      </c>
+      <c r="J59" s="9">
+        <v>38.729999999999997</v>
+      </c>
+      <c r="K59" s="9">
+        <v>1229.27</v>
+      </c>
+      <c r="L59" s="9">
+        <v>429.58</v>
+      </c>
+      <c r="M59" s="9">
+        <v>235.92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="12">
+        <v>704010042</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="9">
+        <v>8133</v>
+      </c>
+      <c r="D60" s="9">
+        <v>8186</v>
+      </c>
+      <c r="E60" s="2">
+        <v>8133</v>
+      </c>
+      <c r="F60" s="2">
+        <v>8159</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" s="12">
+        <v>704010042</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C61" s="9">
         <v>9115</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D61" s="9">
         <v>9141</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E61" s="1">
         <v>9115</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F61" s="1">
         <v>9141</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G61" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="H61" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I61" s="9">
         <v>478.87</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J61" s="9">
         <v>288.73</v>
       </c>
-      <c r="K59" s="9">
+      <c r="K61" s="9">
         <v>725.35</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L61" s="9">
         <v>556.34</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="I60" s="9">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I62" s="9">
         <v>7</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J62" s="9">
         <v>63</v>
       </c>
-      <c r="K60" s="9">
+      <c r="K62" s="9">
         <v>273</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L62" s="9">
         <v>333</v>
       </c>
-      <c r="M60" s="9">
+      <c r="M62" s="9">
         <v>530</v>
       </c>
-      <c r="N60" s="9">
+      <c r="N62" s="9">
         <v>600</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
-        <v>703010131</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C61" s="9">
-        <v>1255</v>
-      </c>
-      <c r="D61" s="9">
-        <v>1308</v>
-      </c>
-      <c r="E61" s="2">
-        <v>1255</v>
-      </c>
-      <c r="F61" s="2">
-        <v>1281</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="I61" s="9">
-        <v>3.65</v>
-      </c>
-      <c r="J61" s="9">
-        <v>328.57</v>
-      </c>
-      <c r="K61" s="9">
-        <v>1583.24</v>
-      </c>
-      <c r="L61" s="9">
-        <v>2136.58</v>
-      </c>
-      <c r="M61" s="9">
-        <v>2502.34</v>
-      </c>
-      <c r="N61" s="9">
-        <v>2427.3200000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
-        <v>703010131</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="9">
-        <v>5855</v>
-      </c>
-      <c r="D62" s="9">
-        <v>5908</v>
-      </c>
-      <c r="E62" s="2">
-        <v>5885</v>
-      </c>
-      <c r="F62" s="2">
-        <v>5911</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -2855,22 +2898,43 @@
         <v>703010131</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C63" s="9">
-        <v>5942</v>
+        <v>1255</v>
       </c>
       <c r="D63" s="9">
-        <v>5971</v>
-      </c>
-      <c r="E63" s="1">
-        <v>5942</v>
-      </c>
-      <c r="F63" s="1">
-        <v>5971</v>
+        <v>1308</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1255</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1281</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I63" s="9">
+        <v>3.65</v>
+      </c>
+      <c r="J63" s="9">
+        <v>328.57</v>
+      </c>
+      <c r="K63" s="9">
+        <v>1583.24</v>
+      </c>
+      <c r="L63" s="9">
+        <v>2136.58</v>
+      </c>
+      <c r="M63" s="9">
+        <v>2502.34</v>
+      </c>
+      <c r="N63" s="9">
+        <v>2427.3200000000002</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -2878,201 +2942,205 @@
         <v>703010131</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C64" s="9">
-        <v>8349</v>
+        <v>5855</v>
       </c>
       <c r="D64" s="9">
-        <v>8402</v>
+        <v>5908</v>
       </c>
       <c r="E64" s="2">
-        <v>8361</v>
+        <v>5885</v>
       </c>
       <c r="F64" s="2">
-        <v>8387</v>
+        <v>5911</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>136</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>703010131</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C65" s="9">
-        <v>6324</v>
+        <v>5942</v>
       </c>
       <c r="D65" s="9">
-        <v>6377</v>
-      </c>
-      <c r="E65" s="2">
-        <v>6330</v>
-      </c>
-      <c r="F65" s="2">
-        <v>6356</v>
+        <v>5971</v>
+      </c>
+      <c r="E65" s="1">
+        <v>5942</v>
+      </c>
+      <c r="F65" s="1">
+        <v>5971</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>138</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>703010131</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="9">
+        <v>8349</v>
+      </c>
+      <c r="D66" s="9">
+        <v>8402</v>
+      </c>
+      <c r="E66" s="2">
+        <v>8361</v>
+      </c>
+      <c r="F66" s="2">
+        <v>8387</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>703010131</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="9">
+        <v>6324</v>
+      </c>
+      <c r="D67" s="9">
+        <v>6377</v>
+      </c>
+      <c r="E67" s="2">
+        <v>6330</v>
+      </c>
+      <c r="F67" s="2">
+        <v>6356</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>703010131</v>
+      </c>
+      <c r="B68" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C68" s="9">
         <v>8986</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D68" s="9">
         <v>9018</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E68" s="1">
         <v>8986</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F68" s="1">
         <v>9018</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="G68" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="H68" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I66" s="9">
+      <c r="I68" s="9">
         <v>1823.57</v>
       </c>
-      <c r="J66" s="9">
+      <c r="J68" s="9">
         <v>257.14</v>
       </c>
-      <c r="K66" s="9">
+      <c r="K68" s="9">
         <v>205.08</v>
       </c>
-      <c r="L66" s="9">
+      <c r="L68" s="9">
         <v>195.94</v>
       </c>
-      <c r="M66" s="9">
+      <c r="M68" s="9">
         <v>78.680000000000007</v>
       </c>
-      <c r="N66" s="9">
+      <c r="N68" s="9">
         <v>60.41</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="I67" s="9">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="I69" s="9">
         <v>32</v>
       </c>
-      <c r="J67" s="9">
+      <c r="J69" s="9">
         <v>39</v>
       </c>
-      <c r="K67" s="9">
+      <c r="K69" s="9">
         <v>54</v>
       </c>
-      <c r="L67" s="9">
+      <c r="L69" s="9">
         <v>81</v>
       </c>
-      <c r="M67" s="9">
+      <c r="M69" s="9">
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="9">
-        <v>706010164</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" s="9">
-        <v>1663</v>
-      </c>
-      <c r="D68" s="9">
-        <v>1716</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1663</v>
-      </c>
-      <c r="F68" s="2">
-        <v>1689</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" s="9">
-        <v>706010164</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="9">
-        <v>1855</v>
-      </c>
-      <c r="D69" s="9">
-        <v>1908</v>
-      </c>
-      <c r="E69" s="2">
-        <v>1882</v>
-      </c>
-      <c r="F69" s="2">
-        <v>1908</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
         <v>706010164</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="C70" s="9">
-        <v>1978</v>
+        <v>1663</v>
       </c>
       <c r="D70" s="9">
-        <v>2031</v>
+        <v>1716</v>
       </c>
       <c r="E70" s="2">
-        <v>1978</v>
+        <v>1663</v>
       </c>
       <c r="F70" s="2">
-        <v>2010</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>146</v>
-      </c>
+        <v>1689</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
         <v>706010164</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C71" s="9">
-        <v>4365</v>
+        <v>1855</v>
       </c>
       <c r="D71" s="9">
-        <v>4418</v>
+        <v>1908</v>
       </c>
       <c r="E71" s="2">
-        <v>4383</v>
+        <v>1882</v>
       </c>
       <c r="F71" s="2">
-        <v>4412</v>
+        <v>1908</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -3080,22 +3148,22 @@
         <v>706010164</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C72" s="9">
-        <v>5900</v>
+        <v>1978</v>
       </c>
       <c r="D72" s="9">
-        <v>5926</v>
-      </c>
-      <c r="E72" s="1">
-        <v>5900</v>
-      </c>
-      <c r="F72" s="1">
-        <v>5926</v>
+        <v>2031</v>
+      </c>
+      <c r="E72" s="2">
+        <v>1978</v>
+      </c>
+      <c r="F72" s="2">
+        <v>2010</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -3103,172 +3171,172 @@
         <v>706010164</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C73" s="9">
-        <v>6849</v>
+        <v>4365</v>
       </c>
       <c r="D73" s="9">
-        <v>6875</v>
-      </c>
-      <c r="E73" s="1">
-        <v>6849</v>
-      </c>
-      <c r="F73" s="1">
-        <v>6875</v>
+        <v>4418</v>
+      </c>
+      <c r="E73" s="2">
+        <v>4383</v>
+      </c>
+      <c r="F73" s="2">
+        <v>4412</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="J73"/>
+        <v>148</v>
+      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
         <v>706010164</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C74" s="9">
-        <v>7005</v>
+        <v>5900</v>
       </c>
       <c r="D74" s="9">
-        <v>7058</v>
-      </c>
-      <c r="E74" s="2">
-        <v>7026</v>
-      </c>
-      <c r="F74" s="2">
-        <v>7055</v>
+        <v>5926</v>
+      </c>
+      <c r="E74" s="1">
+        <v>5900</v>
+      </c>
+      <c r="F74" s="1">
+        <v>5926</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="J74"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="9">
         <v>706010164</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C75" s="9">
-        <v>8986</v>
+        <v>6849</v>
       </c>
       <c r="D75" s="9">
-        <v>9018</v>
+        <v>6875</v>
       </c>
       <c r="E75" s="1">
-        <v>8986</v>
+        <v>6849</v>
       </c>
       <c r="F75" s="1">
-        <v>9018</v>
+        <v>6875</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I75" s="9">
-        <v>1381.11</v>
-      </c>
-      <c r="J75" s="14">
-        <v>4863.12</v>
-      </c>
-      <c r="K75" s="9">
-        <v>4662.88</v>
-      </c>
-      <c r="L75" s="9">
-        <v>5525.4</v>
-      </c>
-      <c r="M75" s="9">
-        <v>4560.58</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J75"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
         <v>706010164</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C76" s="9">
-        <v>9109</v>
+        <v>7005</v>
       </c>
       <c r="D76" s="9">
-        <v>9141</v>
-      </c>
-      <c r="E76" s="1">
-        <v>9109</v>
-      </c>
-      <c r="F76" s="1">
-        <v>9141</v>
+        <v>7058</v>
+      </c>
+      <c r="E76" s="2">
+        <v>7026</v>
+      </c>
+      <c r="F76" s="2">
+        <v>7055</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J76"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" s="9">
+        <v>706010164</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" s="9">
+        <v>8986</v>
+      </c>
+      <c r="D77" s="9">
+        <v>9018</v>
+      </c>
+      <c r="E77" s="1">
+        <v>8986</v>
+      </c>
+      <c r="F77" s="1">
+        <v>9018</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="I77" s="9">
-        <v>29</v>
-      </c>
-      <c r="J77" s="9">
-        <v>71</v>
+        <v>1381.11</v>
+      </c>
+      <c r="J77" s="14">
+        <v>4863.12</v>
       </c>
       <c r="K77" s="9">
-        <v>154</v>
+        <v>4662.88</v>
       </c>
       <c r="L77" s="9">
-        <v>592</v>
+        <v>5525.4</v>
+      </c>
+      <c r="M77" s="9">
+        <v>4560.58</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
-        <v>700010058</v>
+        <v>706010164</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="C78" s="9">
-        <v>1228</v>
+        <v>9109</v>
       </c>
       <c r="D78" s="9">
-        <v>1254</v>
-      </c>
-      <c r="E78" s="6">
-        <v>1228</v>
-      </c>
-      <c r="F78" s="6">
-        <v>1254</v>
+        <v>9141</v>
+      </c>
+      <c r="E78" s="1">
+        <v>9109</v>
+      </c>
+      <c r="F78" s="1">
+        <v>9141</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>1</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="J78"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A79" s="9">
-        <v>700010058</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C79" s="9">
-        <v>1273</v>
-      </c>
-      <c r="D79" s="9">
-        <v>1305</v>
-      </c>
-      <c r="E79" s="6">
-        <v>1273</v>
-      </c>
-      <c r="F79" s="6">
-        <v>1305</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>3</v>
+      <c r="I79" s="9">
+        <v>29</v>
+      </c>
+      <c r="J79" s="9">
+        <v>71</v>
+      </c>
+      <c r="K79" s="9">
+        <v>154</v>
+      </c>
+      <c r="L79" s="9">
+        <v>592</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -3276,37 +3344,22 @@
         <v>700010058</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C80" s="9">
-        <v>1507</v>
+        <v>1228</v>
       </c>
       <c r="D80" s="9">
-        <v>1536</v>
+        <v>1254</v>
       </c>
       <c r="E80" s="6">
-        <v>1507</v>
+        <v>1228</v>
       </c>
       <c r="F80" s="6">
-        <v>1536</v>
+        <v>1254</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="I80" s="9">
-        <v>89.33</v>
-      </c>
-      <c r="J80" s="9">
-        <v>337.4</v>
-      </c>
-      <c r="K80" s="9">
-        <v>169.07</v>
-      </c>
-      <c r="L80" s="9">
-        <v>106.14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -3314,124 +3367,133 @@
         <v>700010058</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="C81" s="9">
-        <v>3834</v>
+        <v>1273</v>
       </c>
       <c r="D81" s="9">
-        <v>3860</v>
-      </c>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
+        <v>1305</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1273</v>
+      </c>
+      <c r="F81" s="6">
+        <v>1305</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
         <v>700010058</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>161</v>
+        <v>4</v>
       </c>
       <c r="C82" s="9">
-        <v>9142</v>
+        <v>1507</v>
       </c>
       <c r="D82" s="9">
-        <v>9168</v>
+        <v>1536</v>
       </c>
       <c r="E82" s="6">
-        <v>9142</v>
+        <v>1507</v>
       </c>
       <c r="F82" s="6">
-        <v>9168</v>
+        <v>1536</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="I82" s="9">
+        <v>89.33</v>
+      </c>
+      <c r="J82" s="9">
+        <v>337.4</v>
+      </c>
+      <c r="K82" s="9">
+        <v>169.07</v>
+      </c>
+      <c r="L82" s="9">
+        <v>106.14</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I83" s="9">
-        <v>12</v>
-      </c>
-      <c r="J83" s="9">
-        <v>30</v>
-      </c>
-      <c r="K83" s="9">
-        <v>303</v>
-      </c>
-      <c r="L83" s="9">
-        <v>466</v>
-      </c>
-      <c r="M83" s="9">
-        <v>588</v>
-      </c>
+      <c r="A83" s="9">
+        <v>700010058</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="9">
+        <v>3834</v>
+      </c>
+      <c r="D83" s="9">
+        <v>3860</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
-        <v>703010159</v>
+        <v>700010058</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C84" s="9">
-        <v>1327</v>
+        <v>9142</v>
       </c>
       <c r="D84" s="9">
-        <v>1353</v>
+        <v>9168</v>
       </c>
       <c r="E84" s="6">
-        <v>1327</v>
+        <v>9142</v>
       </c>
       <c r="F84" s="6">
-        <v>1353</v>
+        <v>9168</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
-        <v>703010159</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C85" s="9">
-        <v>1711</v>
-      </c>
-      <c r="D85" s="9">
-        <v>1764</v>
-      </c>
-      <c r="E85" s="8">
-        <v>1732</v>
-      </c>
-      <c r="F85" s="8">
-        <v>1758</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>166</v>
+        <v>700010058</v>
+      </c>
+      <c r="E85" s="16">
+        <v>7974</v>
+      </c>
+      <c r="F85" s="16">
+        <v>8000</v>
+      </c>
+      <c r="G85" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A86" s="9">
-        <v>703010159</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C86" s="9">
-        <v>2556</v>
-      </c>
-      <c r="D86" s="9">
-        <v>2585</v>
-      </c>
-      <c r="E86" s="6">
-        <v>2556</v>
-      </c>
-      <c r="F86" s="6">
-        <v>2585</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>168</v>
+      <c r="I86" s="9">
+        <v>12</v>
+      </c>
+      <c r="J86" s="9">
+        <v>30</v>
+      </c>
+      <c r="K86" s="9">
+        <v>303</v>
+      </c>
+      <c r="L86" s="9">
+        <v>466</v>
+      </c>
+      <c r="M86" s="9">
+        <v>588</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -3439,22 +3501,22 @@
         <v>703010159</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C87" s="9">
-        <v>5631</v>
+        <v>1327</v>
       </c>
       <c r="D87" s="9">
-        <v>5684</v>
-      </c>
-      <c r="E87" s="8">
-        <v>5658</v>
-      </c>
-      <c r="F87" s="8">
-        <v>5684</v>
+        <v>1353</v>
+      </c>
+      <c r="E87" s="6">
+        <v>1327</v>
+      </c>
+      <c r="F87" s="6">
+        <v>1353</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -3462,37 +3524,22 @@
         <v>703010159</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C88" s="9">
-        <v>8495</v>
+        <v>1711</v>
       </c>
       <c r="D88" s="9">
-        <v>8548</v>
+        <v>1764</v>
       </c>
       <c r="E88" s="8">
-        <v>8130</v>
+        <v>1732</v>
       </c>
       <c r="F88" s="8">
-        <v>8156</v>
+        <v>1758</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H88" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="I88" s="9">
-        <v>2.56</v>
-      </c>
-      <c r="J88" s="9">
-        <v>62.95</v>
-      </c>
-      <c r="K88" s="9">
-        <v>18.350000000000001</v>
-      </c>
-      <c r="M88" s="9">
-        <v>125.2</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -3500,22 +3547,22 @@
         <v>703010159</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C89" s="9">
-        <v>8109</v>
+        <v>2556</v>
       </c>
       <c r="D89" s="9">
-        <v>8186</v>
-      </c>
-      <c r="E89" s="8">
-        <v>8501</v>
-      </c>
-      <c r="F89" s="8">
-        <v>8527</v>
+        <v>2585</v>
+      </c>
+      <c r="E89" s="6">
+        <v>2556</v>
+      </c>
+      <c r="F89" s="6">
+        <v>2585</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -3523,185 +3570,217 @@
         <v>703010159</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C90" s="9">
-        <v>9325</v>
+        <v>5631</v>
       </c>
       <c r="D90" s="9">
-        <v>9378</v>
+        <v>5684</v>
       </c>
       <c r="E90" s="8">
-        <v>9328</v>
+        <v>5658</v>
       </c>
       <c r="F90" s="8">
-        <v>9354</v>
+        <v>5684</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H90" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="I90" s="9">
-        <v>79.67</v>
-      </c>
-      <c r="J90" s="9">
-        <v>88.97</v>
-      </c>
-      <c r="K90" s="9">
-        <v>127.06</v>
-      </c>
-      <c r="L90" s="9">
-        <v>80.599999999999994</v>
-      </c>
-      <c r="M90" s="9">
-        <v>74.099999999999994</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="9">
+        <v>703010159</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="9">
+        <v>8495</v>
+      </c>
+      <c r="D91" s="9">
+        <v>8548</v>
+      </c>
+      <c r="E91" s="8">
+        <v>8130</v>
+      </c>
+      <c r="F91" s="8">
+        <v>8156</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I91" s="9">
+        <v>2.56</v>
+      </c>
+      <c r="J91" s="9">
+        <v>62.95</v>
+      </c>
+      <c r="K91" s="9">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="M91" s="9">
+        <v>125.2</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="9">
-        <v>700010607</v>
+        <v>703010159</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C92" s="9">
-        <v>1000</v>
+        <v>8109</v>
       </c>
       <c r="D92" s="9">
-        <v>1026</v>
-      </c>
+        <v>8186</v>
+      </c>
+      <c r="E92" s="8">
+        <v>8501</v>
+      </c>
+      <c r="F92" s="8">
+        <v>8527</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H92" s="13"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="9">
+        <v>703010159</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="9">
+        <v>9325</v>
+      </c>
+      <c r="D93" s="9">
+        <v>9378</v>
+      </c>
+      <c r="E93" s="8">
+        <v>9328</v>
+      </c>
+      <c r="F93" s="8">
+        <v>9354</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I93" s="9">
+        <v>79.67</v>
+      </c>
+      <c r="J93" s="9">
+        <v>88.97</v>
+      </c>
+      <c r="K93" s="9">
+        <v>127.06</v>
+      </c>
+      <c r="L93" s="9">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="M93" s="9">
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="9">
         <v>700010607</v>
       </c>
-      <c r="B93" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C93" s="9">
-        <v>1327</v>
-      </c>
-      <c r="D93" s="9">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A94" s="9">
-        <v>700010607</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C94" s="9">
-        <v>8736</v>
-      </c>
-      <c r="D94" s="9">
-        <v>8786</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I95" s="9">
-        <v>11</v>
-      </c>
-      <c r="J95" s="9">
-        <v>18</v>
-      </c>
-      <c r="K95" s="9">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="12">
-        <v>705010185</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C96" s="9">
-        <v>1000</v>
-      </c>
-      <c r="D96" s="9">
-        <v>1026</v>
-      </c>
-      <c r="E96" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F96" s="1">
-        <v>1026</v>
-      </c>
-      <c r="G96" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="H96" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="I96" s="9">
-        <v>98.8</v>
-      </c>
-      <c r="J96" s="9">
-        <v>0</v>
-      </c>
-      <c r="K96" s="9">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="B95" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95">
+        <v>9109</v>
+      </c>
+      <c r="F95">
+        <v>9141</v>
+      </c>
+      <c r="G95" t="s">
+        <v>192</v>
+      </c>
+      <c r="H95" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="12">
         <v>705010185</v>
       </c>
       <c r="B97" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D97" s="9">
+        <v>1026</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F97" s="1">
+        <v>1026</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="I97" s="9">
+        <v>98.8</v>
+      </c>
+      <c r="J97" s="9">
+        <v>0</v>
+      </c>
+      <c r="K97" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="12">
+        <v>705010185</v>
+      </c>
+      <c r="B98" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C98" s="9">
         <v>1327</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D98" s="9">
         <v>1353</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E98" s="1">
         <v>1327</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F98" s="1">
         <v>1353</v>
       </c>
-      <c r="G97" s="9" t="s">
+      <c r="G98" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I98" s="9">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I99" s="9">
         <v>11</v>
       </c>
-      <c r="J98" s="9">
+      <c r="J99" s="9">
         <v>32</v>
       </c>
-      <c r="K98" s="9">
+      <c r="K99" s="9">
         <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="9">
-        <v>705010198</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" s="9">
-        <v>1507</v>
-      </c>
-      <c r="D99" s="9">
-        <v>1536</v>
-      </c>
-      <c r="E99" s="6">
-        <v>1507</v>
-      </c>
-      <c r="F99" s="6">
-        <v>1536</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -3709,33 +3788,56 @@
         <v>705010198</v>
       </c>
       <c r="B100" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="9">
+        <v>1507</v>
+      </c>
+      <c r="D100" s="9">
+        <v>1536</v>
+      </c>
+      <c r="E100" s="6">
+        <v>1507</v>
+      </c>
+      <c r="F100" s="6">
+        <v>1536</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="9">
+        <v>705010198</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C101" s="9">
         <v>9040</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D101" s="9">
         <v>9066</v>
       </c>
-      <c r="E100" s="6">
+      <c r="E101" s="6">
         <v>9040</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F101" s="6">
         <v>9066</v>
       </c>
-      <c r="G100" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H100" s="9" t="s">
+      <c r="G101" t="s">
+        <v>183</v>
+      </c>
+      <c r="H101" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I100" s="9">
+      <c r="I101" s="9">
         <v>0</v>
       </c>
-      <c r="J100" s="9">
+      <c r="J101" s="9">
         <v>118.85</v>
       </c>
-      <c r="K100" s="9">
+      <c r="K101" s="9">
         <v>384.55</v>
       </c>
     </row>

</xml_diff>